<commit_message>
Győri telephely alap config
</commit_message>
<xml_diff>
--- a/IP címek.xlsx
+++ b/IP címek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Informatikai-rendszer-es-alkalmazas-uzemelteto-technikusi-vizgsa-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064FAA72-44F5-42F9-8E77-31976FE53379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333556A9-5B5C-4479-89D3-B6FC93A42881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BUDAPESTI KÖZPONT" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="228">
   <si>
     <t>IP CÍM</t>
   </si>
@@ -353,9 +353,6 @@
     <t>192.150.0.172</t>
   </si>
   <si>
-    <t>192.150.174</t>
-  </si>
-  <si>
     <t>192.150.0.169</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>192.150.0.12</t>
   </si>
   <si>
-    <t>192.150.0.100</t>
-  </si>
-  <si>
     <t>192.150.0.5</t>
   </si>
   <si>
@@ -383,9 +377,6 @@
     <t>192.150.0.164</t>
   </si>
   <si>
-    <t>192.150.0.166</t>
-  </si>
-  <si>
     <t>192.150.0.161</t>
   </si>
   <si>
@@ -696,6 +687,33 @@
   </si>
   <si>
     <t>192.100.30.13</t>
+  </si>
+  <si>
+    <t>HSRP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VTP </t>
+  </si>
+  <si>
+    <t>DOMAIN</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>gls.hu</t>
+  </si>
+  <si>
+    <t>gls1234</t>
+  </si>
+  <si>
+    <t>192.150.0.14</t>
+  </si>
+  <si>
+    <t>192.150.0.165</t>
+  </si>
+  <si>
+    <t>192.150.173</t>
   </si>
 </sst>
 </file>
@@ -1058,51 +1076,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1129,6 +1102,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -1506,7 +1524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B9:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -1531,14 +1549,14 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="54" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>0</v>
@@ -1554,15 +1572,15 @@
       </c>
     </row>
     <row r="10" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="51" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>40</v>
@@ -1571,7 +1589,7 @@
         <v>71</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="33" t="s">
         <v>37</v>
       </c>
       <c r="N10" s="2" t="s">
@@ -1585,13 +1603,13 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>40</v>
@@ -1600,7 +1618,7 @@
         <v>71</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="49"/>
+      <c r="I11" s="34"/>
       <c r="M11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1615,8 +1633,8 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="43"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1648,7 @@
         <v>71</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="49"/>
+      <c r="I12" s="34"/>
       <c r="M12" s="3" t="s">
         <v>42</v>
       </c>
@@ -1645,8 +1663,8 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="46"/>
-      <c r="C13" s="43"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="25" t="s">
         <v>25</v>
       </c>
@@ -1660,11 +1678,11 @@
         <v>71</v>
       </c>
       <c r="H13" s="25"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="53" t="s">
+      <c r="I13" s="34"/>
+      <c r="J13" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="K13" s="54"/>
+      <c r="K13" s="39"/>
       <c r="M13" s="3" t="s">
         <v>43</v>
       </c>
@@ -1679,8 +1697,8 @@
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="46"/>
-      <c r="C14" s="43"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="25" t="s">
         <v>26</v>
       </c>
@@ -1694,9 +1712,9 @@
         <v>71</v>
       </c>
       <c r="H14" s="25"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="54"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
       <c r="M14" s="3" t="s">
         <v>44</v>
       </c>
@@ -1711,8 +1729,8 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="43"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="25" t="s">
         <v>27</v>
       </c>
@@ -1726,20 +1744,20 @@
         <v>71</v>
       </c>
       <c r="H15" s="25"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" s="54"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="39"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="46"/>
-      <c r="C16" s="43"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>40</v>
@@ -1748,13 +1766,13 @@
         <v>71</v>
       </c>
       <c r="H16" s="5"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="46"/>
-      <c r="C17" s="44"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="6" t="s">
         <v>29</v>
       </c>
@@ -1768,22 +1786,22 @@
         <v>71</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="53" t="s">
+      <c r="I17" s="35"/>
+      <c r="J17" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="54"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="2:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="55"/>
+      <c r="C18" s="48" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>40</v>
@@ -1792,7 +1810,7 @@
         <v>72</v>
       </c>
       <c r="H18" s="11"/>
-      <c r="I18" s="51" t="s">
+      <c r="I18" s="36" t="s">
         <v>38</v>
       </c>
       <c r="M18" s="3" t="s">
@@ -1809,8 +1827,8 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="40"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="4" t="s">
         <v>16</v>
       </c>
@@ -1824,7 +1842,7 @@
         <v>72</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="34"/>
       <c r="M19" s="9" t="s">
         <v>51</v>
       </c>
@@ -1839,13 +1857,13 @@
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="40"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="49"/>
       <c r="D20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>40</v>
@@ -1854,7 +1872,7 @@
         <v>72</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="49"/>
+      <c r="I20" s="34"/>
       <c r="M20" s="9" t="s">
         <v>52</v>
       </c>
@@ -1869,13 +1887,13 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="40"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>40</v>
@@ -1884,11 +1902,11 @@
         <v>72</v>
       </c>
       <c r="H21" s="7"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="53" t="s">
+      <c r="I21" s="34"/>
+      <c r="J21" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="K21" s="54"/>
+      <c r="K21" s="39"/>
       <c r="M21" s="9" t="s">
         <v>53</v>
       </c>
@@ -1900,8 +1918,8 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="40"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="49"/>
       <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1915,9 +1933,9 @@
         <v>72</v>
       </c>
       <c r="H22" s="5"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="39"/>
       <c r="M22" s="9" t="s">
         <v>54</v>
       </c>
@@ -1929,8 +1947,8 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="46"/>
-      <c r="C23" s="40"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="4" t="s">
         <v>20</v>
       </c>
@@ -1944,11 +1962,11 @@
         <v>72</v>
       </c>
       <c r="H23" s="7"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="54"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" s="39"/>
       <c r="M23" s="9" t="s">
         <v>46</v>
       </c>
@@ -1956,13 +1974,13 @@
       <c r="O23" s="7"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="40"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="49"/>
       <c r="D24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>40</v>
@@ -1971,18 +1989,18 @@
         <v>72</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="54"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="39"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="46"/>
-      <c r="C25" s="40"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>40</v>
@@ -1991,20 +2009,20 @@
         <v>72</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="53" t="s">
+      <c r="I25" s="34"/>
+      <c r="J25" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="K25" s="54"/>
+      <c r="K25" s="39"/>
     </row>
     <row r="26" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="46"/>
-      <c r="C26" s="40"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>40</v>
@@ -2013,7 +2031,7 @@
         <v>72</v>
       </c>
       <c r="H26" s="5"/>
-      <c r="I26" s="49"/>
+      <c r="I26" s="34"/>
       <c r="M26" s="3" t="s">
         <v>50</v>
       </c>
@@ -2028,8 +2046,8 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="46"/>
-      <c r="C27" s="41"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="12" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2061,7 @@
         <v>72</v>
       </c>
       <c r="H27" s="13"/>
-      <c r="I27" s="50"/>
+      <c r="I27" s="35"/>
       <c r="M27" s="9" t="s">
         <v>51</v>
       </c>
@@ -2058,15 +2076,15 @@
       </c>
     </row>
     <row r="28" spans="2:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="46"/>
-      <c r="C28" s="36" t="s">
+      <c r="B28" s="55"/>
+      <c r="C28" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>40</v>
@@ -2075,13 +2093,13 @@
         <v>73</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="51" t="s">
+      <c r="I28" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="J28" s="55" t="s">
+      <c r="J28" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="K28" s="56"/>
+      <c r="K28" s="41"/>
       <c r="M28" s="9" t="s">
         <v>52</v>
       </c>
@@ -2096,8 +2114,8 @@
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="46"/>
-      <c r="C29" s="37"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="46"/>
       <c r="D29" s="25" t="s">
         <v>30</v>
       </c>
@@ -2111,11 +2129,11 @@
         <v>73</v>
       </c>
       <c r="H29" s="25"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K29" s="54"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" s="39"/>
       <c r="M29" s="9" t="s">
         <v>53</v>
       </c>
@@ -2127,13 +2145,13 @@
       </c>
     </row>
     <row r="30" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="46"/>
-      <c r="C30" s="38"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="47"/>
       <c r="D30" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>40</v>
@@ -2142,11 +2160,11 @@
         <v>73</v>
       </c>
       <c r="H30" s="14"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="53" t="s">
+      <c r="I30" s="35"/>
+      <c r="J30" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K30" s="54"/>
+      <c r="K30" s="39"/>
       <c r="M30" s="9" t="s">
         <v>54</v>
       </c>
@@ -2158,8 +2176,8 @@
       </c>
     </row>
     <row r="31" spans="2:16" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="46"/>
-      <c r="C31" s="33" t="s">
+      <c r="B31" s="55"/>
+      <c r="C31" s="42" t="s">
         <v>6</v>
       </c>
       <c r="D31" s="10" t="s">
@@ -2175,8 +2193,8 @@
         <v>74</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="51" t="s">
-        <v>127</v>
+      <c r="I31" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>46</v>
@@ -2185,8 +2203,8 @@
       <c r="O31" s="7"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="46"/>
-      <c r="C32" s="34"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="4" t="s">
         <v>32</v>
       </c>
@@ -2200,15 +2218,15 @@
         <v>74</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="53" t="s">
+      <c r="I32" s="34"/>
+      <c r="J32" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="K32" s="54"/>
+      <c r="K32" s="39"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="46"/>
-      <c r="C33" s="34"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="4" t="s">
         <v>33</v>
       </c>
@@ -2222,13 +2240,13 @@
         <v>74</v>
       </c>
       <c r="H33" s="7"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="53"/>
-      <c r="K33" s="54"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="39"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="46"/>
-      <c r="C34" s="34"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="4" t="s">
         <v>34</v>
       </c>
@@ -2242,15 +2260,15 @@
         <v>74</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="54"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" s="39"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="46"/>
-      <c r="C35" s="34"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="4" t="s">
         <v>35</v>
       </c>
@@ -2264,13 +2282,13 @@
         <v>74</v>
       </c>
       <c r="H35" s="7"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="54"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="39"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="47"/>
-      <c r="C36" s="35"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="4" t="s">
         <v>36</v>
       </c>
@@ -2284,14 +2302,19 @@
         <v>74</v>
       </c>
       <c r="H36" s="5"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="53" t="s">
+      <c r="I36" s="37"/>
+      <c r="J36" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K36" s="54"/>
+      <c r="K36" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C18:C27"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="B9:B36"/>
     <mergeCell ref="I10:I17"/>
     <mergeCell ref="I18:I27"/>
     <mergeCell ref="I28:I30"/>
@@ -2308,11 +2331,6 @@
     <mergeCell ref="J25:K25"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="J36:K36"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C18:C27"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="B9:B36"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2322,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77FF8342-E713-4ECC-957D-961FCC53A967}">
-  <dimension ref="B5:P31"/>
+  <dimension ref="B5:P36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,7 +2354,7 @@
     <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
     <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
@@ -2355,10 +2373,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
@@ -2403,16 +2421,16 @@
       <c r="B10" s="58"/>
       <c r="C10" s="64"/>
       <c r="D10" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>97</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="60"/>
@@ -2420,7 +2438,7 @@
         <v>97</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N10" s="5" t="s">
         <v>103</v>
@@ -2442,10 +2460,10 @@
       <c r="H11" s="21"/>
       <c r="I11" s="60"/>
       <c r="M11" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>95</v>
@@ -2464,10 +2482,10 @@
       <c r="H12" s="28"/>
       <c r="I12" s="60"/>
       <c r="M12" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O12" s="5" t="s">
         <v>95</v>
@@ -2480,24 +2498,24 @@
       <c r="B13" s="58"/>
       <c r="C13" s="64"/>
       <c r="D13" s="29" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>97</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="60"/>
       <c r="M13" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>95</v>
@@ -2530,16 +2548,16 @@
       <c r="B16" s="58"/>
       <c r="C16" s="64"/>
       <c r="D16" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>117</v>
+        <v>226</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>97</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="60"/>
@@ -2552,9 +2570,9 @@
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="48"/>
+      <c r="I17" s="33"/>
       <c r="M17" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>0</v>
@@ -2572,16 +2590,16 @@
         <v>4</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>93</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="61" t="s">
@@ -2594,7 +2612,7 @@
         <v>51</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>93</v>
@@ -2607,16 +2625,16 @@
       <c r="B19" s="58"/>
       <c r="C19" s="67"/>
       <c r="D19" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="60"/>
@@ -2627,7 +2645,7 @@
         <v>52</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>97</v>
@@ -2640,16 +2658,16 @@
       <c r="B20" s="58"/>
       <c r="C20" s="67"/>
       <c r="D20" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>93</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="60"/>
@@ -2657,7 +2675,7 @@
         <v>53</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>97</v>
@@ -2667,16 +2685,16 @@
       <c r="B21" s="58"/>
       <c r="C21" s="67"/>
       <c r="D21" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>93</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="60"/>
@@ -2684,7 +2702,7 @@
         <v>54</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O21" s="5" t="s">
         <v>95</v>
@@ -2694,16 +2712,16 @@
       <c r="B22" s="58"/>
       <c r="C22" s="68"/>
       <c r="D22" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>93</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="62"/>
@@ -2719,7 +2737,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E23" s="11" t="s">
         <v>106</v>
@@ -2728,7 +2746,7 @@
         <v>97</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="61" t="s">
@@ -2742,7 +2760,7 @@
       <c r="B24" s="58"/>
       <c r="C24" s="70"/>
       <c r="D24" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>106</v>
@@ -2751,7 +2769,7 @@
         <v>97</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="60"/>
@@ -2763,21 +2781,21 @@
       <c r="B25" s="58"/>
       <c r="C25" s="70"/>
       <c r="D25" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>97</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="48"/>
+      <c r="I25" s="33"/>
       <c r="M25" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>0</v>
@@ -2795,7 +2813,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>104</v>
@@ -2807,8 +2825,8 @@
         <v>100</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="51" t="s">
-        <v>127</v>
+      <c r="I26" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="J26" t="s">
         <v>94</v>
@@ -2817,7 +2835,7 @@
         <v>51</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>93</v>
@@ -2830,7 +2848,7 @@
       <c r="B27" s="58"/>
       <c r="C27" s="72"/>
       <c r="D27" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>101</v>
@@ -2842,7 +2860,7 @@
         <v>100</v>
       </c>
       <c r="H27" s="5"/>
-      <c r="I27" s="49"/>
+      <c r="I27" s="34"/>
       <c r="J27" t="s">
         <v>95</v>
       </c>
@@ -2850,7 +2868,7 @@
         <v>52</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="O27" s="5" t="s">
         <v>97</v>
@@ -2863,7 +2881,7 @@
       <c r="B28" s="58"/>
       <c r="C28" s="72"/>
       <c r="D28" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>102</v>
@@ -2875,12 +2893,12 @@
         <v>100</v>
       </c>
       <c r="H28" s="7"/>
-      <c r="I28" s="49"/>
+      <c r="I28" s="34"/>
       <c r="M28" s="9" t="s">
         <v>53</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>97</v>
@@ -2890,10 +2908,10 @@
       <c r="B29" s="58"/>
       <c r="C29" s="72"/>
       <c r="D29" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>95</v>
@@ -2902,12 +2920,12 @@
         <v>100</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="49"/>
+      <c r="I29" s="34"/>
       <c r="M29" s="9" t="s">
         <v>54</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O29" s="5" t="s">
         <v>95</v>
@@ -2917,7 +2935,7 @@
       <c r="B30" s="58"/>
       <c r="C30" s="72"/>
       <c r="D30" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>99</v>
@@ -2929,7 +2947,7 @@
         <v>100</v>
       </c>
       <c r="H30" s="7"/>
-      <c r="I30" s="49"/>
+      <c r="I30" s="34"/>
       <c r="M30" s="9" t="s">
         <v>46</v>
       </c>
@@ -2940,7 +2958,7 @@
       <c r="B31" s="59"/>
       <c r="C31" s="73"/>
       <c r="D31" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>105</v>
@@ -2952,7 +2970,63 @@
         <v>100</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="52"/>
+      <c r="I31" s="37"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="M32" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M33" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2974,10 +3048,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B959F40D-70A9-47C2-99A0-8342AE521164}">
-  <dimension ref="B8:P31"/>
+  <dimension ref="B8:P35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2997,13 +3071,13 @@
   <sheetData>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="57" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
@@ -3045,30 +3119,30 @@
       <c r="B10" s="58"/>
       <c r="C10" s="78"/>
       <c r="D10" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="60"/>
       <c r="M10" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>40</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -3081,16 +3155,16 @@
       <c r="H11" s="21"/>
       <c r="I11" s="60"/>
       <c r="M11" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -3103,46 +3177,46 @@
       <c r="H12" s="28"/>
       <c r="I12" s="60"/>
       <c r="M12" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="O12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="58"/>
       <c r="C13" s="78"/>
       <c r="D13" s="29" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>40</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H13" s="28"/>
       <c r="I13" s="60"/>
       <c r="M13" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="O13" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P13" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
@@ -3169,16 +3243,16 @@
       <c r="B16" s="58"/>
       <c r="C16" s="78"/>
       <c r="D16" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>40</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="60"/>
@@ -3191,9 +3265,9 @@
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="48"/>
+      <c r="I17" s="33"/>
       <c r="M17" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>0</v>
@@ -3211,16 +3285,16 @@
         <v>4</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>40</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="61" t="s">
@@ -3230,29 +3304,29 @@
         <v>51</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="58"/>
       <c r="C19" s="81"/>
       <c r="D19" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="60"/>
@@ -3260,29 +3334,29 @@
         <v>52</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>40</v>
       </c>
       <c r="P19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="58"/>
       <c r="C20" s="81"/>
       <c r="D20" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E20" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="60"/>
@@ -3290,7 +3364,7 @@
         <v>53</v>
       </c>
       <c r="N20" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O20" s="7" t="s">
         <v>40</v>
@@ -3300,16 +3374,16 @@
       <c r="B21" s="58"/>
       <c r="C21" s="81"/>
       <c r="D21" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="60"/>
@@ -3317,7 +3391,7 @@
         <v>54</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="O21" s="5" t="s">
         <v>40</v>
@@ -3327,16 +3401,16 @@
       <c r="B22" s="58"/>
       <c r="C22" s="82"/>
       <c r="D22" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>40</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="62"/>
@@ -3352,16 +3426,16 @@
         <v>5</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>40</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="61" t="s">
@@ -3372,16 +3446,16 @@
       <c r="B24" s="58"/>
       <c r="C24" s="84"/>
       <c r="D24" s="25" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F24" s="25" t="s">
         <v>40</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="60"/>
@@ -3390,21 +3464,21 @@
       <c r="B25" s="58"/>
       <c r="C25" s="85"/>
       <c r="D25" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>40</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="62"/>
       <c r="M25" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>0</v>
@@ -3422,48 +3496,48 @@
         <v>6</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>40</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H26" s="15"/>
       <c r="I26" s="74" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>51</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>40</v>
       </c>
       <c r="P26" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="58"/>
       <c r="C27" s="72"/>
       <c r="D27" s="4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="75"/>
@@ -3471,29 +3545,29 @@
         <v>52</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="O27" s="5" t="s">
         <v>40</v>
       </c>
       <c r="P27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="58"/>
       <c r="C28" s="72"/>
       <c r="D28" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="75"/>
@@ -3501,7 +3575,7 @@
         <v>53</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>40</v>
@@ -3511,16 +3585,16 @@
       <c r="B29" s="58"/>
       <c r="C29" s="72"/>
       <c r="D29" s="4" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="75"/>
@@ -3528,7 +3602,7 @@
         <v>54</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="O29" s="5" t="s">
         <v>40</v>
@@ -3538,16 +3612,16 @@
       <c r="B30" s="58"/>
       <c r="C30" s="72"/>
       <c r="D30" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="75"/>
@@ -3561,19 +3635,39 @@
       <c r="B31" s="59"/>
       <c r="C31" s="73"/>
       <c r="D31" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>40</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="76"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>224</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>